<commit_message>
Updated literature review results
</commit_message>
<xml_diff>
--- a/lit-review/DL4SE lit review.xlsx
+++ b/lit-review/DL4SE lit review.xlsx
@@ -8,17 +8,17 @@
     <sheet state="visible" name="summery" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_DB979693_5E90_4AB3_98AE_60188F13C1E9_.wvu.FilterData">Papers!$D$1:$E$1007</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_132F2CAA_BF36_43D0_B9A7_20FD098DF28A_.wvu.FilterData">Papers!$D$1:$E$1007</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{DB979693-5E90-4AB3-98AE-60188F13C1E9}" name="Code and data"/>
+    <customWorkbookView activeSheetId="0" maximized="1" tabRatio="600" windowHeight="0" windowWidth="0" guid="{132F2CAA-BF36-43D0-B9A7-20FD098DF28A}" name="Code and data"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="286">
   <si>
     <t>Number</t>
   </si>
@@ -860,6 +860,15 @@
     <t>https://www.researchgate.net/publication/318873760_Easy_over_hard_a_case_study_on_deep_learning</t>
   </si>
   <si>
+    <t>Improving Deep Learning for Defect Prediction (using the GHOST Hyperparameter Optimizer)</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2008.03835</t>
+  </si>
+  <si>
+    <t>epsilon dom</t>
+  </si>
+  <si>
     <t>Just-In-Time Defect Identification and Localization: A Two-Phase Framework</t>
   </si>
   <si>
@@ -873,7 +882,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -949,10 +958,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="10.0"/>
-      <name val="Helvetica Neue"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1011,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1092,9 +1097,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1700,7 +1702,7 @@
       </c>
       <c r="L4" s="3">
         <f>COUNTIFS(E2:E1007, "=Yes", F2:F1007, "=Yes")</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -7411,10 +7413,10 @@
       <c r="C121" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="D121" s="32" t="s">
+      <c r="D121" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E121" s="32" t="s">
+      <c r="E121" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F121" s="2" t="s">
@@ -7488,7 +7490,7 @@
       <c r="AD122" s="3"/>
     </row>
     <row r="123">
-      <c r="A123" s="32">
+      <c r="A123" s="2">
         <v>105.0</v>
       </c>
       <c r="B123" s="31" t="s">
@@ -7497,25 +7499,25 @@
       <c r="C123" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="D123" s="32" t="s">
+      <c r="D123" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E123" s="32" t="s">
+      <c r="E123" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F123" s="32" t="s">
+      <c r="F123" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G123" s="32" t="s">
+      <c r="G123" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H123" s="32" t="s">
+      <c r="H123" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="I123" s="32" t="s">
+      <c r="I123" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="J123" s="32" t="s">
+      <c r="J123" s="2" t="s">
         <v>24</v>
       </c>
       <c r="K123" s="3"/>
@@ -7540,16 +7542,36 @@
       <c r="AD123" s="3"/>
     </row>
     <row r="124">
-      <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
-      <c r="G124" s="3"/>
-      <c r="H124" s="3"/>
-      <c r="I124" s="32"/>
-      <c r="J124" s="3"/>
+      <c r="A124" s="2">
+        <v>106.0</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I124" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
       <c r="M124" s="3"/>
@@ -35829,7 +35851,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DB979693-5E90-4AB3-98AE-60188F13C1E9}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{132F2CAA-BF36-43D0-B9A7-20FD098DF28A}" filter="1" showAutoFilter="1">
       <autoFilter ref="$D$1:$E$1007">
         <filterColumn colId="0">
           <filters>
@@ -35949,8 +35971,9 @@
     <hyperlink r:id="rId102" ref="C120"/>
     <hyperlink r:id="rId103" ref="C121"/>
     <hyperlink r:id="rId104" ref="C123"/>
+    <hyperlink r:id="rId105" ref="C124"/>
   </hyperlinks>
-  <drawing r:id="rId105"/>
+  <drawing r:id="rId106"/>
 </worksheet>
 </file>
 
@@ -35966,10 +35989,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>14</v>
@@ -36007,7 +36030,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2">
@@ -36016,12 +36039,12 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>17</v>
       </c>
     </row>
@@ -36031,12 +36054,12 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="32" t="s">
         <v>17</v>
       </c>
     </row>
@@ -36051,77 +36074,77 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="33" t="s">
+      <c r="A20" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="33" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="33" t="s">
+      <c r="A23" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="34" t="s">
         <v>17</v>
       </c>
     </row>
@@ -36141,117 +36164,117 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="34" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="34" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="32" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="33" t="s">
+      <c r="A32" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="33" t="s">
+      <c r="A33" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="32" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="33" t="s">
+      <c r="A38" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="32" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="32" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="33" t="s">
+      <c r="A43" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="33" t="s">
+      <c r="A46" s="32" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="33" t="s">
+      <c r="A47" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="33" t="s">
+      <c r="A48" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="33" t="s">
+      <c r="A49" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="33" t="s">
+      <c r="A50" s="32" t="s">
         <v>17</v>
       </c>
     </row>
@@ -36261,72 +36284,72 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="36" t="s">
+      <c r="A52" s="35" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="33" t="s">
+      <c r="A53" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="33" t="s">
+      <c r="A55" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="33" t="s">
+      <c r="A56" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="33" t="s">
+      <c r="A57" s="32" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="33" t="s">
+      <c r="A58" s="32" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="33" t="s">
+      <c r="A59" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="33" t="s">
+      <c r="A60" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="33" t="s">
+      <c r="A61" s="32" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="33" t="s">
+      <c r="A62" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="33" t="s">
+      <c r="A63" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="33" t="s">
+      <c r="A64" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="33" t="s">
+      <c r="A65" s="32" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>